<commit_message>
[FIX] fix enum values in test data
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SnapeN\Dev\funding-service-design-post-award-data-store\core\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01630D5-BA97-4C1E-A832-8E9B00B17DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDDD93F-C2EC-4013-886C-5CFB029F218F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2085" windowWidth="37275" windowHeight="14040" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Dim" sheetId="1" r:id="rId1"/>
@@ -710,36 +710,15 @@
     <t>RiskOwnerRole</t>
   </si>
   <si>
-    <t>2 - Medium</t>
-  </si>
-  <si>
-    <t>1 - Low</t>
-  </si>
-  <si>
-    <t>2 - Distant: next 12 months</t>
-  </si>
-  <si>
     <t>Rising Costs</t>
   </si>
   <si>
-    <t>3 - High</t>
-  </si>
-  <si>
-    <t>3 - Medium impact</t>
-  </si>
-  <si>
-    <t>1 - Remote</t>
-  </si>
-  <si>
     <t>Lorem Ipsum</t>
   </si>
   <si>
     <t>Cost and availability of materials</t>
   </si>
   <si>
-    <t>3 - Approaching: next 6 months</t>
-  </si>
-  <si>
     <t>Jane Doe, Head of Property Services</t>
   </si>
   <si>
@@ -806,10 +785,31 @@
     <t>Fake Council Name</t>
   </si>
   <si>
-    <t>4 - Significant impact</t>
-  </si>
-  <si>
-    <t>2 - Low impact</t>
+    <t>3. Approaching: next 6 months</t>
+  </si>
+  <si>
+    <t>1. Remote</t>
+  </si>
+  <si>
+    <t>2. Medium</t>
+  </si>
+  <si>
+    <t>3. Medium Impact</t>
+  </si>
+  <si>
+    <t>2. Low Impact</t>
+  </si>
+  <si>
+    <t>4. Significant Impact</t>
+  </si>
+  <si>
+    <t>3. High</t>
+  </si>
+  <si>
+    <t>1. Low</t>
+  </si>
+  <si>
+    <t>2. Distant: next 12 months</t>
   </si>
 </sst>
 </file>
@@ -2108,7 +2108,7 @@
         <v>44651</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>54</v>
@@ -2131,7 +2131,7 @@
         <v>44834</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>54</v>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>108</v>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>108</v>
@@ -2736,7 +2736,7 @@
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>108</v>
@@ -2744,7 +2744,7 @@
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>108</v>
@@ -2899,7 +2899,7 @@
         <v>65</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3592,7 +3592,7 @@
         <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3608,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3676,40 +3676,40 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3717,40 +3717,40 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>223</v>
+        <v>254</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3758,40 +3758,40 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3860,19 +3860,19 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3892,7 +3892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3921,13 +3921,13 @@
     </row>
     <row r="2" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D2" s="1">
         <v>123456789</v>
@@ -3968,7 +3968,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[#PAB-273] endpoints use sql db as backend
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDDD93F-C2EC-4013-886C-5CFB029F218F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5CCEEA-D459-4470-8DE9-6B2A3EB11DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2085" windowWidth="37275" windowHeight="14040" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27075" yWindow="3840" windowWidth="24495" windowHeight="16290" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Dim" sheetId="1" r:id="rId1"/>
@@ -2267,8 +2267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2333,10 +2333,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="3">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="C3" s="3">
-        <v>44104</v>
+        <v>44134</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>63</v>
@@ -2345,7 +2345,7 @@
         <v>62</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -3608,7 +3608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[#PAB-340] fix alignment of enum values with data model
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
+++ b/tests/controller_tests/resources/DLUCH_Data_Model_V3.4_EXAMPLE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5CCEEA-D459-4470-8DE9-6B2A3EB11DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE1AF69-1107-41EE-AA43-C926A497E125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27075" yWindow="3840" windowWidth="24495" windowHeight="16290" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="5370" windowWidth="38700" windowHeight="15435" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Dim" sheetId="1" r:id="rId1"/>
@@ -785,31 +785,31 @@
     <t>Fake Council Name</t>
   </si>
   <si>
-    <t>3. Approaching: next 6 months</t>
-  </si>
-  <si>
-    <t>1. Remote</t>
-  </si>
-  <si>
-    <t>2. Medium</t>
-  </si>
-  <si>
-    <t>3. Medium Impact</t>
-  </si>
-  <si>
-    <t>2. Low Impact</t>
-  </si>
-  <si>
-    <t>4. Significant Impact</t>
-  </si>
-  <si>
-    <t>3. High</t>
-  </si>
-  <si>
-    <t>1. Low</t>
-  </si>
-  <si>
-    <t>2. Distant: next 12 months</t>
+    <t>1 - Low</t>
+  </si>
+  <si>
+    <t>1 - Remote</t>
+  </si>
+  <si>
+    <t>2 - Medium</t>
+  </si>
+  <si>
+    <t>2 - Low Impact</t>
+  </si>
+  <si>
+    <t>2 - Distant: next 12 months</t>
+  </si>
+  <si>
+    <t>3 - High</t>
+  </si>
+  <si>
+    <t>3 - Medium Impact</t>
+  </si>
+  <si>
+    <t>3 - Approaching: next 6 months</t>
+  </si>
+  <si>
+    <t>4 - Significant Impact</t>
   </si>
 </sst>
 </file>
@@ -2267,7 +2267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -3608,8 +3608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3691,22 +3691,22 @@
         <v>31</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>233</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>225</v>
@@ -3732,7 +3732,7 @@
         <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>249</v>
@@ -3741,10 +3741,10 @@
         <v>234</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>248</v>
@@ -3773,22 +3773,22 @@
         <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>235</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>249</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>231</v>

</xml_diff>